<commit_message>
fixing + add most relevant tickets / testing_copy_filter.py / v.9.12
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -411,7 +411,27 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>SPL</t>
         </is>
       </c>
     </row>
@@ -582,6 +602,524 @@
       <c r="C12" t="inlineStr">
         <is>
           <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11:14:51</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11:14:58</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Top cover</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11:15:32</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Tornillo atascado en tolva</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11:15:35</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11:16:16</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Colisión placas</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11:16:21</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Error en sensor de salida</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>11:16:23</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Marco atascado en parte inferior</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11:16:32</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Colisión placas</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11:24:41</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Cover atascado</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11:24:44</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>No coloca bien la pcb</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:24:48</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>NOK Soldadura Plástico</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:24:50</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Fallo cámara cover</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:24:53</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Fallo cámara QR</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>11:24:55</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>No coloca bien foam</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updating interface / testing_copy_filter.py / v.9.15
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1123,6 +1123,857 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>11:28:32</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>11:31:03</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>11:31:07</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foams</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>11:31:09</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>11:35:04</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>11:35:08</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>11:35:10</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Fallo cámara visión</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>11:35:13</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>11:35:16</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>11:35:24</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>AOI no detecta pieza</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>11:35:49</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Fallo fijador tapa</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>11:35:51</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Fallo fijador tapa</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>11:35:54</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Fallo fijador tapa</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>11:35:56</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Fallo fijador tapa</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>11:36:02</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>11:36:07</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>11:36:14</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>11:36:22</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>11:36:30</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>11:36:34</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>11:45:45</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Tornillo atascado</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>11:45:47</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>11:45:51</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>No lee QR</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more ideas - v.9.25
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1974,6 +1974,80 @@
         </is>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>12:11:17</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Power CP</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>12:11:20</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new test - new interface / fixing tickets / confirmed tickets / v.10.0
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,13 @@
           <t>SPL</t>
         </is>
       </c>
-    </row>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Hora de Reparación</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -2045,6 +2051,342 @@
       <c r="G51" t="inlineStr">
         <is>
           <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>12:21:27</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>12:21:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>12:21:56</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>12:22:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>12:22:37</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>12:22:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>12:22:57</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>12:23:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>12:23:54</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>12:23:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>12:24:03</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Fallo etiqueta</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>12:24:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>12:24:17</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Cámara no detecta busbar</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>12:24:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>12:25:51</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Top cover</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>12:26:01</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
testing_copy_filter.py fixed / new interface / new buttons / implementing new advanced filter for relevant tickets and add details of tickets / v.10.5
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2390,6 +2390,253 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>12:35:28</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>12:35:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>12:37:22</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>12:37:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>12:37:26</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Fallo fijador tapa</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>12:37:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>12:38:22</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Soldadura defectuosa</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>12:38:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>12:38:37</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Marco atascado en parte inferior</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>12:46:36</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>AOI no detecta pieza</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>12:46:48</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more ideas to "text.txt"
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2637,6 +2637,174 @@
         </is>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>12:52:01</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Error en sensor de salida</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>12:52:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>12:52:09</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Sensor de PCB detecta que hay placa cuando no la hay</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>12:52:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>12:52:16</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Fallo dispensación glue</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>12:52:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>12:52:35</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Soldadura defectuosa</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>12:52:39</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update detail window for relevant tickets / v.10.7
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2805,6 +2805,216 @@
         </is>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>12:56:48</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>12:56:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>12:57:05</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>12:57:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>12:57:25</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>12:57:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>12:57:26</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>12:57:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>12:57:28</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>12:57:32</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more ideas / text.txt / v.10.7.5
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,7 +440,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -3014,6 +3013,81 @@
           <t>12:57:32</t>
         </is>
       </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>13:00:36</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>13:00:42</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating excel file / tickets_pideu.xlsx / v.10.8.0
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -440,6 +440,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -3050,6 +3051,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>13:02:12</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3087,7 +3093,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H76" t="inlineStr"/>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>13:02:13</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new visual ticket "fixing" and "confirm" / v.10.9
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,11 @@
           <t>Hora de Reparación</t>
         </is>
       </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Tiempo de Reparación</t>
+        </is>
+      </c>
     </row>
     <row r="2"/>
     <row r="3">
@@ -3096,6 +3101,419 @@
       <c r="H76" t="inlineStr">
         <is>
           <t>13:02:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>09:30:59</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>09:31:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>09:31:18</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>09:31:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>09:38:57</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Tornillo atascado en tolva</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>09:39:06</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>0:00:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>09:39:09</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Fallo etiqueta</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>09:39:21</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>0:00:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>09:39:24</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>09:39:38</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>0:00:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>09:49:49</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>No detecta presencia power CP</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>09:50:01</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>0:00:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>09:49:57</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>09:50:03</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>09:50:18</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Cámara no detecta busbar</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>09:50:27</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>0:00:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>09:50:39</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Top cover</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>09:50:45</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
new json file - add tickets on "Fixing" - "Pendiente" mode / v.10.15
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1225,6 +1225,1302 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11:01:20</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Marco atascado en parte inferior</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>11:01:27</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0:00:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11:02:14</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Fallo dispensación glue</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>11:02:26</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>0:00:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11:02:17</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Error en sensor de salida</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>11:02:27</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>0:00:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:02:20</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Sensor de PCB detecta que hay placa cuando no la hay</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>11:02:28</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>0:00:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:02:23</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Marco atascado en parte inferior</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>11:03:47</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>0:01:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:03:54</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Fallo dispensación glue</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>11:06:56</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>0:03:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>11:09:07</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Soldadura defectuosa</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>11:10:26</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>0:01:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>11:11:32</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>11:13:54</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>0:02:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>11:12:21</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>11:12:29</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>0:00:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>11:24:50</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>NOK Soldad. Plástico+Metal</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>11:26:27</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>0:01:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>11:26:03</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>NOK Soldad. Plástico+Metal</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>11:26:05</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>11:26:06</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Core enganchado</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>11:26:08</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>11:26:09</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Fallo cámara ferrite</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>11:26:11</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>11:26:13</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Pieza enganchada en HV Test</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>11:26:15</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>11:26:19</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>NOK Soldad. Plástico+Metal</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>11:26:31</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>0:00:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>11:26:21</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>No coloca bien foam</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>11:27:39</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>0:01:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>11:26:23</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Repeat funcional</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>11:26:32</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>0:00:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>11:26:25</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Fallo Funcional</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>11:26:32</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>0:00:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>11:26:34</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Repeat funcional</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>11:26:38</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>11:26:36</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Repeat funcional</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>11:26:38</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>11:27:42</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>No coloca bien el core</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>11:30:11</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>0:02:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>11:31:22</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>11:32:55</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>0:01:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>11:31:34</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>11:33:00</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>0:01:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>11:37:56</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>11:40:53</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>0:02:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>11:40:55</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>QR desplazado</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>11:44:08</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>11:56:48</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>11:56:50</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>11:57:48</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>11:57:50</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing beta_test.py / v.10.9
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,7 +445,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -2520,6 +2519,344 @@
           <t>0:00:02</t>
         </is>
       </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>12:27:56</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>12:28:01</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>12:28:00</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Secuencia atornillador</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>12:32:07</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>0:04:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>12:28:17</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>12:32:28</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>0:04:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>12:32:45</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>12:32:52</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>0:00:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>12:42:26</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>12:42:29</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>12:43:36</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>12:43:40</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
error fixed / beta_test.py / v.11.0
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -2855,8 +2856,184 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-05-17</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>09:44:52</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Tornillo atascado</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-05-17</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>09:52:45</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>09:52:51</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-05-17</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>09:53:01</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Screw K30 no lo detecta puesto</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>09:53:09</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>0:00:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-05-17</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>09:53:05</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>No lee QR</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>10:24:34</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>0:31:29</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new structure / beta version / more code organization and clean
</commit_message>
<xml_diff>
--- a/tickets_pideu.xlsx
+++ b/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3035,6 +3035,372 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-05-17</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>10:56:37</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Cámara no detecta busbar</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>10:56:39</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-05-17</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>11:02:43</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>11:02:45</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-05-17</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>11:14:24</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>11:14:25</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-05-17</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>11:16:20</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Screw K30 no lo detecta puesto</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>11:16:22</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-05-17</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>11:16:29</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-05-17</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>11:58:14</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>11:58:18</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2024-05-17</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>11:58:31</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Atasco tuerca</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>12:00:10</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>0:01:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2024-05-17</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>12:02:19</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>12:02:25</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>